<commit_message>
implementacion id y hora entrada corregido
</commit_message>
<xml_diff>
--- a/registros_excel/2024-02-08.xlsx
+++ b/registros_excel/2024-02-08.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,126 +443,227 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Documento</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Nombre</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Vinculo</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Hora Escaneo</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Hora Entrada</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Hora Salida</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Rango</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>10541212</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>prueba Proveedor 2</t>
+          <t>1053868254</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tercero</t>
+          <t>Tatiana Pachon</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>2024-02-08</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>08:25:11</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>08:25:11</t>
+          <t>14:09:27</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>08:25:11</t>
+          <t>14:09:27</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Entrada AM</t>
+          <t>14:09:27</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1054398414</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Julian Largo</t>
+          <t>10267084</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Ruben Lopez</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Administrativa</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>2024-02-08</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>08:26:24</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>08:26:24</t>
+          <t>14:09:39</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>08:26:24</t>
+          <t>14:09:39</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Entrada AM</t>
+          <t>14:09:39</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1053868254</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tatiana Pachon</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-02-08</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>14:12:10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>14:09:27</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>14:12:10</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>10267084</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ruben Lopez</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-02-08</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>14:13:08</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>14:09:39</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>14:13:08</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Entrada PM</t>
         </is>
       </c>
     </row>

</xml_diff>